<commit_message>
Added pax in escort
</commit_message>
<xml_diff>
--- a/public/assets/sample-group-list.xlsx
+++ b/public/assets/sample-group-list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\web\GBI-GermanShepard\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web\GBI-GermanShepard\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>first_name</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>mobile</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +385,7 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -399,6 +402,9 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>